<commit_message>
Updated models and student answers
</commit_message>
<xml_diff>
--- a/data/models/questions-skill-model1a_leak.xlsx
+++ b/data/models/questions-skill-model1a_leak.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgia/repositories/virtual-CAT-itas/data/old_posteriors/target_skills/models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgia/repositories/bn-based-learning-networks-with-noisy-gates/data/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B4E7D3-43CE-EA49-BFBB-5A40C1B5DD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442B9A81-52DD-1547-9E5E-F7E788DFAFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="3200" windowWidth="29040" windowHeight="16000" xr2:uid="{3D5E00E8-EA45-C34D-85AA-17AD78DA61C2}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>0D VS</t>
   </si>
   <si>
-    <t>OD V</t>
-  </si>
-  <si>
     <t>1D VSF</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>Extra</t>
+  </si>
+  <si>
+    <t>0D V</t>
   </si>
 </sst>
 </file>
@@ -357,6 +357,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -368,15 +377,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,7 +707,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M83" sqref="M83"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,34 +720,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="31"/>
       <c r="M1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="21">
         <v>0</v>
       </c>
@@ -778,9 +778,9 @@
       <c r="M2"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="20" t="s">
         <v>13</v>
       </c>
@@ -788,67 +788,67 @@
         <v>14</v>
       </c>
       <c r="F3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="I3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="J3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="K3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="L3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="M3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="18" t="s">
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="20" t="s">
+      <c r="E4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="F4" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="G4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="H4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="I4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="J4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="K4" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="L4" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="24" t="s">
-        <v>31</v>
-      </c>
       <c r="M4" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29">
+      <c r="A5" s="26">
         <v>1</v>
       </c>
       <c r="B5" s="4">
@@ -889,7 +889,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="5">
         <v>2</v>
       </c>
@@ -928,7 +928,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="5">
         <v>3</v>
       </c>
@@ -967,7 +967,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="5">
         <v>4</v>
       </c>
@@ -1006,7 +1006,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="5">
         <v>5</v>
       </c>
@@ -1045,7 +1045,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="5">
         <v>6</v>
       </c>
@@ -1084,7 +1084,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="5">
         <v>7</v>
       </c>
@@ -1123,7 +1123,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="5">
         <v>8</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="5">
         <v>9</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30">
+      <c r="A14" s="25">
         <v>2</v>
       </c>
       <c r="B14" s="4">
@@ -1242,7 +1242,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="5">
         <v>2</v>
       </c>
@@ -1281,7 +1281,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="5">
         <v>3</v>
       </c>
@@ -1320,7 +1320,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="29"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="5">
         <v>4</v>
       </c>
@@ -1359,7 +1359,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="29"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="5">
         <v>5</v>
       </c>
@@ -1398,7 +1398,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="5">
         <v>6</v>
       </c>
@@ -1437,7 +1437,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="5">
         <v>7</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="5">
         <v>8</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="6">
         <v>9</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29">
+      <c r="A23" s="26">
         <v>3</v>
       </c>
       <c r="B23" s="5">
@@ -1595,7 +1595,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="29"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="5">
         <v>2</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="5">
         <v>3</v>
       </c>
@@ -1673,7 +1673,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="5">
         <v>4</v>
       </c>
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="5">
         <v>5</v>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="5">
         <v>6</v>
       </c>
@@ -1790,7 +1790,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="5">
         <v>7</v>
       </c>
@@ -1829,7 +1829,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="5">
         <v>8</v>
       </c>
@@ -1868,7 +1868,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="5">
         <v>9</v>
       </c>
@@ -1907,7 +1907,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="30">
+      <c r="A32" s="25">
         <v>4</v>
       </c>
       <c r="B32" s="4">
@@ -1948,7 +1948,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="29"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="5">
         <v>2</v>
       </c>
@@ -1987,7 +1987,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="29"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="5">
         <v>3</v>
       </c>
@@ -2026,7 +2026,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="29"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="5">
         <v>4</v>
       </c>
@@ -2065,7 +2065,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="29"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="5">
         <v>5</v>
       </c>
@@ -2104,7 +2104,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="29"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="5">
         <v>6</v>
       </c>
@@ -2143,7 +2143,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="29"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="5">
         <v>7</v>
       </c>
@@ -2182,7 +2182,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="29"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="5">
         <v>8</v>
       </c>
@@ -2221,7 +2221,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="31"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="6">
         <v>9</v>
       </c>
@@ -2260,7 +2260,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="29">
+      <c r="A41" s="26">
         <v>5</v>
       </c>
       <c r="B41" s="5">
@@ -2301,7 +2301,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="29"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="5">
         <v>2</v>
       </c>
@@ -2340,7 +2340,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="29"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="5">
         <v>3</v>
       </c>
@@ -2379,7 +2379,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="29"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="5">
         <v>4</v>
       </c>
@@ -2418,7 +2418,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="29"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="5">
         <v>5</v>
       </c>
@@ -2457,7 +2457,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="29"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="5">
         <v>6</v>
       </c>
@@ -2496,7 +2496,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="29"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="5">
         <v>7</v>
       </c>
@@ -2535,7 +2535,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="29"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="5">
         <v>8</v>
       </c>
@@ -2574,7 +2574,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="29"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="5">
         <v>9</v>
       </c>
@@ -2613,7 +2613,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="30">
+      <c r="A50" s="25">
         <v>6</v>
       </c>
       <c r="B50" s="4">
@@ -2654,7 +2654,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="29"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="5">
         <v>2</v>
       </c>
@@ -2693,7 +2693,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="29"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="5">
         <v>3</v>
       </c>
@@ -2732,7 +2732,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="29"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="5">
         <v>4</v>
       </c>
@@ -2771,7 +2771,7 @@
       </c>
     </row>
     <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="29"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="5">
         <v>5</v>
       </c>
@@ -2810,7 +2810,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="29"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="5">
         <v>6</v>
       </c>
@@ -2849,7 +2849,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="29"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="5">
         <v>7</v>
       </c>
@@ -2888,7 +2888,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="29"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="5">
         <v>8</v>
       </c>
@@ -2927,7 +2927,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="31"/>
+      <c r="A58" s="27"/>
       <c r="B58" s="6">
         <v>9</v>
       </c>
@@ -2966,7 +2966,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="29">
+      <c r="A59" s="26">
         <v>7</v>
       </c>
       <c r="B59" s="5">
@@ -3007,7 +3007,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="29"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="5">
         <v>2</v>
       </c>
@@ -3046,7 +3046,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="29"/>
+      <c r="A61" s="26"/>
       <c r="B61" s="5">
         <v>3</v>
       </c>
@@ -3085,7 +3085,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="29"/>
+      <c r="A62" s="26"/>
       <c r="B62" s="5">
         <v>4</v>
       </c>
@@ -3124,7 +3124,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="29"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="5">
         <v>5</v>
       </c>
@@ -3163,7 +3163,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="29"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="5">
         <v>6</v>
       </c>
@@ -3202,7 +3202,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="29"/>
+      <c r="A65" s="26"/>
       <c r="B65" s="5">
         <v>7</v>
       </c>
@@ -3241,7 +3241,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="29"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="5">
         <v>8</v>
       </c>
@@ -3280,7 +3280,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="29"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="5">
         <v>9</v>
       </c>
@@ -3319,7 +3319,7 @@
       </c>
     </row>
     <row r="68" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="30">
+      <c r="A68" s="25">
         <v>8</v>
       </c>
       <c r="B68" s="4">
@@ -3360,7 +3360,7 @@
       </c>
     </row>
     <row r="69" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="29"/>
+      <c r="A69" s="26"/>
       <c r="B69" s="5">
         <v>2</v>
       </c>
@@ -3399,7 +3399,7 @@
       </c>
     </row>
     <row r="70" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="29"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="5">
         <v>3</v>
       </c>
@@ -3438,7 +3438,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="29"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="5">
         <v>4</v>
       </c>
@@ -3477,7 +3477,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="29"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="5">
         <v>5</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="29"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="5">
         <v>6</v>
       </c>
@@ -3555,7 +3555,7 @@
       </c>
     </row>
     <row r="74" spans="1:13" s="3" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="29"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="5">
         <v>7</v>
       </c>
@@ -3594,7 +3594,7 @@
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A75" s="29"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="5">
         <v>8</v>
       </c>
@@ -3633,7 +3633,7 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A76" s="31"/>
+      <c r="A76" s="27"/>
       <c r="B76" s="6">
         <v>9</v>
       </c>
@@ -3672,7 +3672,7 @@
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A77" s="29">
+      <c r="A77" s="26">
         <v>9</v>
       </c>
       <c r="B77" s="5">
@@ -3713,7 +3713,7 @@
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A78" s="29"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="5">
         <v>2</v>
       </c>
@@ -3752,7 +3752,7 @@
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A79" s="29"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="5">
         <v>3</v>
       </c>
@@ -3791,7 +3791,7 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A80" s="29"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="5">
         <v>4</v>
       </c>
@@ -3830,7 +3830,7 @@
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A81" s="29"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="5">
         <v>5</v>
       </c>
@@ -3869,7 +3869,7 @@
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A82" s="29"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="5">
         <v>6</v>
       </c>
@@ -3908,7 +3908,7 @@
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A83" s="29"/>
+      <c r="A83" s="26"/>
       <c r="B83" s="5">
         <v>7</v>
       </c>
@@ -3947,7 +3947,7 @@
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A84" s="29"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="5">
         <v>8</v>
       </c>
@@ -3986,7 +3986,7 @@
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A85" s="29"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="5">
         <v>9</v>
       </c>
@@ -4025,7 +4025,7 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A86" s="30">
+      <c r="A86" s="25">
         <v>10</v>
       </c>
       <c r="B86" s="4">
@@ -4066,7 +4066,7 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A87" s="29"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="5">
         <v>2</v>
       </c>
@@ -4105,7 +4105,7 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A88" s="29"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="5">
         <v>3</v>
       </c>
@@ -4144,7 +4144,7 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A89" s="29"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="5">
         <v>4</v>
       </c>
@@ -4183,7 +4183,7 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A90" s="29"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="5">
         <v>5</v>
       </c>
@@ -4222,7 +4222,7 @@
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A91" s="29"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="5">
         <v>6</v>
       </c>
@@ -4261,7 +4261,7 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A92" s="29"/>
+      <c r="A92" s="26"/>
       <c r="B92" s="5">
         <v>7</v>
       </c>
@@ -4300,7 +4300,7 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A93" s="29"/>
+      <c r="A93" s="26"/>
       <c r="B93" s="5">
         <v>8</v>
       </c>
@@ -4339,7 +4339,7 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A94" s="31"/>
+      <c r="A94" s="27"/>
       <c r="B94" s="6">
         <v>9</v>
       </c>
@@ -4378,7 +4378,7 @@
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A95" s="29">
+      <c r="A95" s="26">
         <v>11</v>
       </c>
       <c r="B95" s="5">
@@ -4419,7 +4419,7 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A96" s="29"/>
+      <c r="A96" s="26"/>
       <c r="B96" s="5">
         <v>2</v>
       </c>
@@ -4458,7 +4458,7 @@
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A97" s="29"/>
+      <c r="A97" s="26"/>
       <c r="B97" s="5">
         <v>3</v>
       </c>
@@ -4497,7 +4497,7 @@
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A98" s="29"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="5">
         <v>4</v>
       </c>
@@ -4536,7 +4536,7 @@
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A99" s="29"/>
+      <c r="A99" s="26"/>
       <c r="B99" s="5">
         <v>5</v>
       </c>
@@ -4575,7 +4575,7 @@
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A100" s="29"/>
+      <c r="A100" s="26"/>
       <c r="B100" s="5">
         <v>6</v>
       </c>
@@ -4614,7 +4614,7 @@
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A101" s="29"/>
+      <c r="A101" s="26"/>
       <c r="B101" s="5">
         <v>7</v>
       </c>
@@ -4653,7 +4653,7 @@
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A102" s="29"/>
+      <c r="A102" s="26"/>
       <c r="B102" s="5">
         <v>8</v>
       </c>
@@ -4692,7 +4692,7 @@
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A103" s="29"/>
+      <c r="A103" s="26"/>
       <c r="B103" s="5">
         <v>9</v>
       </c>
@@ -4731,7 +4731,7 @@
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A104" s="30">
+      <c r="A104" s="25">
         <v>12</v>
       </c>
       <c r="B104" s="4">
@@ -4772,7 +4772,7 @@
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A105" s="29"/>
+      <c r="A105" s="26"/>
       <c r="B105" s="5">
         <v>2</v>
       </c>
@@ -4811,7 +4811,7 @@
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A106" s="29"/>
+      <c r="A106" s="26"/>
       <c r="B106" s="5">
         <v>3</v>
       </c>
@@ -4850,7 +4850,7 @@
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A107" s="29"/>
+      <c r="A107" s="26"/>
       <c r="B107" s="5">
         <v>4</v>
       </c>
@@ -4889,7 +4889,7 @@
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A108" s="29"/>
+      <c r="A108" s="26"/>
       <c r="B108" s="5">
         <v>5</v>
       </c>
@@ -4928,7 +4928,7 @@
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A109" s="29"/>
+      <c r="A109" s="26"/>
       <c r="B109" s="5">
         <v>6</v>
       </c>
@@ -4967,7 +4967,7 @@
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A110" s="29"/>
+      <c r="A110" s="26"/>
       <c r="B110" s="5">
         <v>7</v>
       </c>
@@ -5006,7 +5006,7 @@
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A111" s="29"/>
+      <c r="A111" s="26"/>
       <c r="B111" s="5">
         <v>8</v>
       </c>
@@ -5045,7 +5045,7 @@
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A112" s="31"/>
+      <c r="A112" s="27"/>
       <c r="B112" s="6">
         <v>9</v>
       </c>
@@ -5085,22 +5085,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A68:A76"/>
-    <mergeCell ref="A77:A85"/>
-    <mergeCell ref="A86:A94"/>
-    <mergeCell ref="A95:A103"/>
-    <mergeCell ref="A104:A112"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A5:A13"/>
     <mergeCell ref="A59:A67"/>
     <mergeCell ref="A14:A22"/>
     <mergeCell ref="A23:A31"/>
     <mergeCell ref="A32:A40"/>
     <mergeCell ref="A41:A49"/>
     <mergeCell ref="A50:A58"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="A68:A76"/>
+    <mergeCell ref="A77:A85"/>
+    <mergeCell ref="A86:A94"/>
+    <mergeCell ref="A95:A103"/>
+    <mergeCell ref="A104:A112"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:L112">
     <cfRule type="colorScale" priority="3">

</xml_diff>